<commit_message>
Entrega de documentos Fase 2 Final
</commit_message>
<xml_diff>
--- a/Fase 2/EVIDENCIAS DE PROYECTO/Planilla set de pruebas.xlsx
+++ b/Fase 2/EVIDENCIAS DE PROYECTO/Planilla set de pruebas.xlsx
@@ -594,12 +594,12 @@
     </font>
     <font>
       <color rgb="FF1B1C1D"/>
-      <name val="&quot;Google Sans Text&quot;"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
       <color rgb="FF1B1C1D"/>
-      <name val="&quot;Google Sans Text&quot;"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -757,28 +757,28 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -787,10 +787,10 @@
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -806,45 +806,36 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="8" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
     <xf borderId="8" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -860,32 +851,25 @@
     <xf borderId="8" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1217,36 +1201,36 @@
       <c r="B8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>1.0</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>0.0</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="22">
-        <v>0.8</v>
+      <c r="F8" s="21">
+        <v>1.0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <v>1.0</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>0.0</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="23"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="19" t="s">
@@ -1255,16 +1239,16 @@
       <c r="B10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <v>1.0</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <v>0.0</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="19" t="s">
@@ -1273,16 +1257,16 @@
       <c r="B11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="20">
         <v>1.0</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>0.0</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="24"/>
+      <c r="F11" s="23"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="19" t="s">
@@ -1291,16 +1275,16 @@
       <c r="B12" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>1.0</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>0.0</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="24"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="19" t="s">
@@ -1318,11 +1302,11 @@
       <c r="E13" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="24"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="E14" s="18"/>
-      <c r="F14" s="26"/>
+      <c r="F14" s="25"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
@@ -1338,7 +1322,7 @@
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="26">
         <v>45948.0</v>
       </c>
       <c r="E16" s="1"/>
@@ -1348,7 +1332,7 @@
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="27">
         <v>0.7916666666666666</v>
       </c>
     </row>
@@ -1356,7 +1340,7 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="27">
         <v>0.8333333333333334</v>
       </c>
     </row>
@@ -1365,7 +1349,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="10"/>
@@ -1409,16 +1393,16 @@
       <c r="B22" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>1.0</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="20">
         <v>0.0</v>
       </c>
       <c r="E22" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="21">
         <v>1.0</v>
       </c>
     </row>
@@ -1426,19 +1410,19 @@
       <c r="A23" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="20">
         <v>1.0</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="20">
         <v>0.0</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="24"/>
+      <c r="F23" s="23"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="20" t="s">
@@ -1447,16 +1431,16 @@
       <c r="B24" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="20">
         <v>1.0</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="20">
         <v>0.0</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="24"/>
+      <c r="F24" s="23"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="20" t="s">
@@ -1465,16 +1449,16 @@
       <c r="B25" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="20">
         <v>1.0</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="20">
         <v>0.0</v>
       </c>
       <c r="E25" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="24"/>
+      <c r="F25" s="23"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="20" t="s">
@@ -1483,22 +1467,22 @@
       <c r="B26" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="20">
         <v>1.0</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="20">
         <v>0.0</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="25"/>
+      <c r="F26" s="24"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="E27" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F27" s="26"/>
+      <c r="F27" s="25"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
@@ -1514,7 +1498,7 @@
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="30">
+      <c r="B29" s="29">
         <v>45948.0</v>
       </c>
       <c r="E29" s="1"/>
@@ -1524,7 +1508,7 @@
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="27">
         <v>0.8333333333333334</v>
       </c>
       <c r="F30" s="1"/>
@@ -1533,7 +1517,7 @@
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B31" s="27">
         <v>0.875</v>
       </c>
     </row>
@@ -1542,7 +1526,7 @@
         <v>54</v>
       </c>
       <c r="B32" s="8"/>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="28" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="10"/>
@@ -1550,7 +1534,7 @@
       <c r="F32" s="11"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="31"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="8"/>
       <c r="C33" s="13" t="s">
         <v>8</v>
@@ -1584,16 +1568,16 @@
       <c r="B35" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="21">
+      <c r="C35" s="20">
         <v>1.0</v>
       </c>
-      <c r="D35" s="21">
+      <c r="D35" s="20">
         <v>0.0</v>
       </c>
       <c r="E35" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="21">
         <v>1.0</v>
       </c>
     </row>
@@ -1601,19 +1585,19 @@
       <c r="A36" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="21">
+      <c r="C36" s="20">
         <v>1.0</v>
       </c>
-      <c r="D36" s="21">
+      <c r="D36" s="20">
         <v>0.0</v>
       </c>
       <c r="E36" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="24"/>
+      <c r="F36" s="23"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="20" t="s">
@@ -1622,16 +1606,16 @@
       <c r="B37" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="21">
+      <c r="C37" s="20">
         <v>1.0</v>
       </c>
-      <c r="D37" s="21">
+      <c r="D37" s="20">
         <v>0.0</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="24"/>
+      <c r="F37" s="23"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="20" t="s">
@@ -1640,16 +1624,16 @@
       <c r="B38" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="21">
+      <c r="C38" s="20">
         <v>1.0</v>
       </c>
-      <c r="D38" s="21">
+      <c r="D38" s="20">
         <v>0.0</v>
       </c>
       <c r="E38" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="24"/>
+      <c r="F38" s="23"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="20" t="s">
@@ -1658,22 +1642,22 @@
       <c r="B39" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="21">
+      <c r="C39" s="20">
         <v>1.0</v>
       </c>
-      <c r="D39" s="21">
+      <c r="D39" s="20">
         <v>0.0</v>
       </c>
       <c r="E39" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="F39" s="25"/>
+      <c r="F39" s="24"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="E40" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F40" s="26"/>
+      <c r="F40" s="25"/>
     </row>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1"/>
@@ -2617,21 +2601,21 @@
     <row r="980" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="F35:F39"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="F35:F39"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:F6"/>
+    <mergeCell ref="F8:F13"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="F22:F26"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2660,232 +2644,232 @@
   </cols>
   <sheetData>
     <row r="1" ht="54.75" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="33" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="35" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" ht="66.0" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="39" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="39" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="39" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" ht="46.5" customHeight="1">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="40" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" ht="38.25" customHeight="1">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="39" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" ht="40.5" customHeight="1">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="39" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
     </row>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1"/>
@@ -3890,196 +3874,196 @@
   </cols>
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="34" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" ht="77.25" customHeight="1">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="44" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="44" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="44" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="44" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="44" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="14">
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
     </row>
     <row r="15">
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -5089,200 +5073,200 @@
   </cols>
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="34" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="3" ht="54.75" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="44" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" ht="65.25" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="E4" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="44" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" ht="53.25" customHeight="1">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="44" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="6" ht="53.25" customHeight="1">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="44" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="7" ht="43.5" customHeight="1">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="44" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="14">
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
     </row>
     <row r="15">
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>